<commit_message>
The hardware setup done.
This is a backup after the hardware setup done.
Arc:
1. FreeRTOS tested.
2. Hardware board Dout0 with 8 channels output. (tested with Oscilloscope).
</commit_message>
<xml_diff>
--- a/RoadScannerDocument/template.xlsx
+++ b/RoadScannerDocument/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\OneDrive\Project\Nanfoon\RoadScanner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Atmel Studio\7.0\RoadScannerDataAcquire\RoadScannerDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_4476A007F3F847654B6D28E9B193274BEE81F99A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5CA0DBBB-EAB4-4CDF-952D-E6F45784C9F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA44DA1-A5C8-4990-A4C9-10A703322050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3093,8 +3093,8 @@
   </sheetPr>
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>

</xml_diff>